<commit_message>
Update produtos.xlsx with latest data
</commit_message>
<xml_diff>
--- a/data/produtos.xlsx
+++ b/data/produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\giraffe-autopecas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497A5821-DDFD-459A-9B10-023969153941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE718A-928C-4B7A-AC50-BF15E094365F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EE34329B-7202-468C-80CD-2EB6AA7100B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>imagem</t>
   </si>
@@ -42,9 +42,6 @@
     <t>iwpo003.jpg</t>
   </si>
   <si>
-    <t>IWPO003</t>
-  </si>
-  <si>
     <t>Palio Fire / Siena / Strada 1.4</t>
   </si>
   <si>
@@ -54,27 +51,18 @@
     <t>0280750596.jpg</t>
   </si>
   <si>
-    <t>Uno Celebration / Mobi / Palio 1.4</t>
-  </si>
-  <si>
     <t>600.00</t>
   </si>
   <si>
     <t>iwpo005.jpg</t>
   </si>
   <si>
-    <t>IWPO005</t>
-  </si>
-  <si>
     <t>Fiat Linea 1.9</t>
   </si>
   <si>
     <t>iwpo006.jpg</t>
   </si>
   <si>
-    <t>iwpo006</t>
-  </si>
-  <si>
     <t>GM Celta 1.0</t>
   </si>
   <si>
@@ -84,13 +72,58 @@
     <t>iwpo007.jpg</t>
   </si>
   <si>
-    <t>iwpo007</t>
-  </si>
-  <si>
     <t>GM Cruze 1.4</t>
   </si>
   <si>
     <t>300.00</t>
+  </si>
+  <si>
+    <t>descricao_longa</t>
+  </si>
+  <si>
+    <t>especificacoes</t>
+  </si>
+  <si>
+    <t>estoque</t>
+  </si>
+  <si>
+    <t>Corpo de borboleta completo, com tampa e asas, abre e fecha e foi feita da mais refinada IA. Serve no Palio e vai na Strada tbm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corpinho para o Uno e Mobi, é pequeno igual eles </t>
+  </si>
+  <si>
+    <t>Oxi, existe carro 1.9? Melhor fazer 2.0 logo de uma vez po</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mais um corpo de borboleta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encorpado na borboleta </t>
+  </si>
+  <si>
+    <t>Corpo de Borboleta Fiat Palio</t>
+  </si>
+  <si>
+    <t>Corpo de Borboleta Fiat Uno/Mobi</t>
+  </si>
+  <si>
+    <t>Corpo de Borboleta Fiat Linea</t>
+  </si>
+  <si>
+    <t>Corpo de Borboleta GM Celta</t>
+  </si>
+  <si>
+    <t>Corpo de Borboleta GM Cruze 1.4</t>
+  </si>
+  <si>
+    <t>Motores 1.4</t>
+  </si>
+  <si>
+    <t>Uno Celebration / Mobi / Palio 1.0</t>
+  </si>
+  <si>
+    <t>Motores 1.0</t>
   </si>
 </sst>
 </file>
@@ -456,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E53B7D-9B0A-48C2-AF11-1E084BDA1FF4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,9 +501,12 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,75 +519,120 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>280750596</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>